<commit_message>
updated Databsestructure and Pdlichtenheft
#230
</commit_message>
<xml_diff>
--- a/Documentation/Planung/Datenbankstruktur.xlsx
+++ b/Documentation/Planung/Datenbankstruktur.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>Spieler</t>
   </si>
@@ -226,10 +226,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -515,30 +515,31 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A2:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="L49" sqref="L49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.140625" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -579,16 +580,16 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -627,16 +628,16 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -672,16 +673,16 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -724,16 +725,16 @@
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -747,6 +748,9 @@
       </c>
       <c r="D19" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -772,16 +776,16 @@
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -830,16 +834,16 @@
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -875,16 +879,16 @@
       <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
@@ -920,16 +924,16 @@
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
@@ -968,16 +972,16 @@
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -1013,16 +1017,16 @@
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
@@ -1038,16 +1042,16 @@
       <c r="H43" s="1"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -1068,18 +1072,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A6:H6"/>
     <mergeCell ref="A46:H46"/>
     <mergeCell ref="A42:H42"/>
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="A18:H18"/>
     <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="A34:H34"/>
     <mergeCell ref="A38:H38"/>
-    <mergeCell ref="A6:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated Stabasestruktur added Database template
added types of coloums to Databasestrukture
added Database template fix #230 @0.5h
</commit_message>
<xml_diff>
--- a/Documentation/Planung/Datenbankstruktur.xlsx
+++ b/Documentation/Planung/Datenbankstruktur.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="46">
   <si>
     <t>Spieler</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Logo</t>
   </si>
   <si>
-    <t>LigaID</t>
-  </si>
-  <si>
     <t>Liga</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
     <t>Nutzername</t>
   </si>
   <si>
-    <t>E-Mail</t>
-  </si>
-  <si>
     <t>Manager</t>
   </si>
   <si>
@@ -86,15 +80,9 @@
     <t>Liga_ID</t>
   </si>
   <si>
-    <t>Administrator</t>
-  </si>
-  <si>
     <t>Nutzer_ID</t>
   </si>
   <si>
-    <t>Spielraunde_ID</t>
-  </si>
-  <si>
     <t>Budget</t>
   </si>
   <si>
@@ -156,6 +144,24 @@
   </si>
   <si>
     <t>Preis</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>EMail</t>
+  </si>
+  <si>
+    <t>Administrator_ID</t>
+  </si>
+  <si>
+    <t>Integer (boolean)</t>
+  </si>
+  <si>
+    <t>Marktwert</t>
   </si>
 </sst>
 </file>
@@ -226,10 +232,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -513,33 +519,34 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A2:H47"/>
+  <dimension ref="A2:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="6" max="6" width="17.140625" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -557,15 +564,30 @@
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
@@ -580,16 +602,16 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -602,16 +624,24 @@
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -628,16 +658,16 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -647,15 +677,21 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -673,44 +709,56 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
@@ -725,16 +773,16 @@
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -744,23 +792,33 @@
         <v>2</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -776,52 +834,68 @@
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="A22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
@@ -834,34 +908,40 @@
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="A26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -879,34 +959,40 @@
       <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
+      <c r="A30" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -924,38 +1010,46 @@
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
+      <c r="A34" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
+      <c r="A36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -972,23 +1066,23 @@
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
+      <c r="A38" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>5</v>
@@ -997,9 +1091,15 @@
       <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
+      <c r="A40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -1017,23 +1117,23 @@
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
+      <c r="A42" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>5</v>
@@ -1041,49 +1141,77 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
     </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
+      <c r="A46" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B47" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C47" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D47" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E47" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A46:H46"/>
+    <mergeCell ref="A42:H42"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A38:H38"/>
     <mergeCell ref="A10:H10"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A26:H26"/>
     <mergeCell ref="A30:H30"/>
     <mergeCell ref="A34:H34"/>
     <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A46:H46"/>
-    <mergeCell ref="A42:H42"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A38:H38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated database structure and database dummy
</commit_message>
<xml_diff>
--- a/Documentation/Planung/Datenbankstruktur.xlsx
+++ b/Documentation/Planung/Datenbankstruktur.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="55">
   <si>
     <t>Spieler</t>
   </si>
@@ -180,6 +180,15 @@
   </si>
   <si>
     <t>String</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Heim_Verein_ID</t>
+  </si>
+  <si>
+    <t>Gast_Verein_ID</t>
   </si>
 </sst>
 </file>
@@ -249,14 +258,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -540,10 +549,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A2:H52"/>
+  <dimension ref="A2:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,19 +566,22 @@
     <col min="8" max="8" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -590,7 +602,7 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>40</v>
       </c>
@@ -612,7 +624,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -622,19 +634,22 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -650,7 +665,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
@@ -668,7 +683,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -678,19 +693,22 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -703,7 +721,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -719,7 +737,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -729,19 +747,22 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -761,7 +782,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
@@ -783,7 +804,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -793,19 +814,22 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
@@ -824,7 +848,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>40</v>
       </c>
@@ -844,7 +868,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -854,19 +878,22 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
@@ -892,7 +919,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>40</v>
       </c>
@@ -918,7 +945,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -928,19 +955,22 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
@@ -953,7 +983,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>40</v>
       </c>
@@ -969,7 +999,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -979,19 +1009,22 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -1004,7 +1037,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>40</v>
       </c>
@@ -1020,7 +1053,7 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1030,19 +1063,22 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>21</v>
       </c>
@@ -1058,7 +1094,7 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
@@ -1076,7 +1112,7 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1086,19 +1122,22 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>50</v>
       </c>
@@ -1111,7 +1150,7 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
@@ -1127,7 +1166,7 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1137,19 +1176,22 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>50</v>
       </c>
@@ -1162,7 +1204,7 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>40</v>
       </c>
@@ -1173,36 +1215,39 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>40</v>
       </c>
@@ -1220,62 +1265,62 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2" t="s">
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D51" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F51" s="4" t="s">
+      <c r="D51" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G51" s="4" t="s">
+      <c r="G51" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F52" s="4" t="s">
+      <c r="A52" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G52" s="4" t="s">
+      <c r="G52" s="2" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>